<commit_message>
file format changed for black font
</commit_message>
<xml_diff>
--- a/public/6 R Daily Report.xlsx
+++ b/public/6 R Daily Report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sangbin.whi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyunmyung.kim\workspace\React\exbon-daily-report\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65089A16-134B-4DF3-81ED-0EDA4147901A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC65CE94-4ED2-4690-BF0B-FB646BAA5B12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -116,7 +116,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -149,14 +149,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -692,7 +684,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -786,15 +778,147 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -803,147 +927,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1449,7 +1432,7 @@
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:G21"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1466,110 +1449,110 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="58"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="48"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="41"/>
       <c r="E2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="45"/>
+      <c r="G2" s="38"/>
     </row>
     <row r="3" spans="1:16" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="48"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="41"/>
       <c r="E3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="44" t="s">
+      <c r="F3" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="45"/>
+      <c r="G3" s="38"/>
     </row>
     <row r="4" spans="1:16" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="61" t="s">
+      <c r="B4" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="62"/>
-      <c r="D4" s="63"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="56"/>
       <c r="E4" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="49"/>
-      <c r="G4" s="50"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="43"/>
     </row>
     <row r="5" spans="1:16" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="64"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="66"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="41"/>
       <c r="E5" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="49"/>
-      <c r="G5" s="50"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="43"/>
     </row>
     <row r="6" spans="1:16" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="56"/>
-      <c r="E6" s="69" t="s">
+      <c r="D6" s="49"/>
+      <c r="E6" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="57" t="s">
+      <c r="F6" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="58"/>
+      <c r="G6" s="51"/>
     </row>
     <row r="7" spans="1:16" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="52"/>
-      <c r="B7" s="54"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="47"/>
       <c r="C7" s="28" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="70"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="60"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="53"/>
     </row>
     <row r="8" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="26"/>
@@ -1577,8 +1560,8 @@
       <c r="C8" s="11"/>
       <c r="D8" s="12"/>
       <c r="E8" s="16"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="68"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="72"/>
     </row>
     <row r="9" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="27"/>
@@ -1586,8 +1569,8 @@
       <c r="C9" s="13"/>
       <c r="D9" s="14"/>
       <c r="E9" s="20"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="33"/>
+      <c r="F9" s="78"/>
+      <c r="G9" s="79"/>
       <c r="M9" s="29"/>
     </row>
     <row r="10" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1596,8 +1579,8 @@
       <c r="C10" s="13"/>
       <c r="D10" s="14"/>
       <c r="E10" s="20"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="33"/>
+      <c r="F10" s="78"/>
+      <c r="G10" s="79"/>
     </row>
     <row r="11" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="27"/>
@@ -1605,8 +1588,8 @@
       <c r="C11" s="13"/>
       <c r="D11" s="14"/>
       <c r="E11" s="20"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="33"/>
+      <c r="F11" s="78"/>
+      <c r="G11" s="79"/>
     </row>
     <row r="12" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="27"/>
@@ -1614,8 +1597,8 @@
       <c r="C12" s="13"/>
       <c r="D12" s="14"/>
       <c r="E12" s="20"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="33"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="79"/>
     </row>
     <row r="13" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="27"/>
@@ -1623,8 +1606,8 @@
       <c r="C13" s="13"/>
       <c r="D13" s="14"/>
       <c r="E13" s="20"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="33"/>
+      <c r="F13" s="78"/>
+      <c r="G13" s="79"/>
     </row>
     <row r="14" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="27"/>
@@ -1632,8 +1615,8 @@
       <c r="C14" s="13"/>
       <c r="D14" s="14"/>
       <c r="E14" s="20"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="33"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="79"/>
     </row>
     <row r="15" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="27"/>
@@ -1641,175 +1624,175 @@
       <c r="C15" s="13"/>
       <c r="D15" s="14"/>
       <c r="E15" s="20"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="33"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="79"/>
     </row>
     <row r="16" spans="1:16" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="41"/>
+      <c r="B16" s="34"/>
       <c r="C16" s="15">
         <f>SUM(C8:C15)</f>
         <v>0</v>
       </c>
       <c r="D16" s="32"/>
-      <c r="E16" s="71"/>
-      <c r="F16" s="72"/>
-      <c r="G16" s="73"/>
+      <c r="E16" s="75"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="77"/>
       <c r="N16" s="18"/>
       <c r="O16" s="19"/>
       <c r="P16" s="19"/>
     </row>
     <row r="17" spans="1:14" s="5" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="38"/>
+      <c r="B17" s="81"/>
+      <c r="C17" s="81"/>
+      <c r="D17" s="81"/>
+      <c r="E17" s="81"/>
+      <c r="F17" s="81"/>
+      <c r="G17" s="82"/>
       <c r="N17" s="6"/>
     </row>
     <row r="18" spans="1:14" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="74"/>
-      <c r="B18" s="75"/>
-      <c r="C18" s="75"/>
-      <c r="D18" s="75"/>
-      <c r="E18" s="75"/>
-      <c r="F18" s="75"/>
-      <c r="G18" s="76"/>
+      <c r="A18" s="59"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="61"/>
       <c r="N18" s="6"/>
     </row>
     <row r="19" spans="1:14" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="77"/>
-      <c r="B19" s="78"/>
-      <c r="C19" s="78"/>
-      <c r="D19" s="78"/>
-      <c r="E19" s="78"/>
-      <c r="F19" s="78"/>
-      <c r="G19" s="79"/>
+      <c r="A19" s="62"/>
+      <c r="B19" s="63"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="64"/>
       <c r="N19" s="6"/>
     </row>
     <row r="20" spans="1:14" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="77"/>
-      <c r="B20" s="78"/>
-      <c r="C20" s="78"/>
-      <c r="D20" s="78"/>
-      <c r="E20" s="78"/>
-      <c r="F20" s="78"/>
-      <c r="G20" s="79"/>
+      <c r="A20" s="62"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="64"/>
     </row>
     <row r="21" spans="1:14" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="80"/>
-      <c r="B21" s="81"/>
-      <c r="C21" s="81"/>
-      <c r="D21" s="81"/>
-      <c r="E21" s="81"/>
-      <c r="F21" s="81"/>
-      <c r="G21" s="82"/>
+      <c r="A21" s="65"/>
+      <c r="B21" s="66"/>
+      <c r="C21" s="66"/>
+      <c r="D21" s="66"/>
+      <c r="E21" s="66"/>
+      <c r="F21" s="66"/>
+      <c r="G21" s="67"/>
     </row>
     <row r="22" spans="1:14" s="5" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="38"/>
+      <c r="B22" s="81"/>
+      <c r="C22" s="81"/>
+      <c r="D22" s="81"/>
+      <c r="E22" s="81"/>
+      <c r="F22" s="81"/>
+      <c r="G22" s="82"/>
       <c r="N22" s="6"/>
     </row>
     <row r="23" spans="1:14" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="74"/>
-      <c r="B23" s="75"/>
-      <c r="C23" s="75"/>
-      <c r="D23" s="75"/>
-      <c r="E23" s="75"/>
-      <c r="F23" s="75"/>
-      <c r="G23" s="76"/>
+      <c r="A23" s="59"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="61"/>
       <c r="N23" s="6"/>
     </row>
     <row r="24" spans="1:14" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="77"/>
-      <c r="B24" s="78"/>
-      <c r="C24" s="78"/>
-      <c r="D24" s="78"/>
-      <c r="E24" s="78"/>
-      <c r="F24" s="78"/>
-      <c r="G24" s="79"/>
+      <c r="A24" s="62"/>
+      <c r="B24" s="63"/>
+      <c r="C24" s="63"/>
+      <c r="D24" s="63"/>
+      <c r="E24" s="63"/>
+      <c r="F24" s="63"/>
+      <c r="G24" s="64"/>
     </row>
     <row r="25" spans="1:14" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="77"/>
-      <c r="B25" s="78"/>
-      <c r="C25" s="78"/>
-      <c r="D25" s="78"/>
-      <c r="E25" s="78"/>
-      <c r="F25" s="78"/>
-      <c r="G25" s="79"/>
+      <c r="A25" s="62"/>
+      <c r="B25" s="63"/>
+      <c r="C25" s="63"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="63"/>
+      <c r="F25" s="63"/>
+      <c r="G25" s="64"/>
     </row>
     <row r="26" spans="1:14" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="80"/>
-      <c r="B26" s="81"/>
-      <c r="C26" s="81"/>
-      <c r="D26" s="81"/>
-      <c r="E26" s="81"/>
-      <c r="F26" s="81"/>
-      <c r="G26" s="82"/>
+      <c r="A26" s="65"/>
+      <c r="B26" s="66"/>
+      <c r="C26" s="66"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="66"/>
+      <c r="F26" s="66"/>
+      <c r="G26" s="67"/>
     </row>
     <row r="27" spans="1:14" s="5" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="38"/>
+      <c r="B27" s="81"/>
+      <c r="C27" s="81"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="81"/>
+      <c r="F27" s="81"/>
+      <c r="G27" s="82"/>
       <c r="N27" s="6"/>
     </row>
     <row r="28" spans="1:14" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="74"/>
-      <c r="B28" s="75"/>
-      <c r="C28" s="75"/>
-      <c r="D28" s="75"/>
-      <c r="E28" s="75"/>
-      <c r="F28" s="75"/>
-      <c r="G28" s="76"/>
+      <c r="A28" s="59"/>
+      <c r="B28" s="60"/>
+      <c r="C28" s="60"/>
+      <c r="D28" s="60"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="61"/>
       <c r="N28" s="6"/>
     </row>
     <row r="29" spans="1:14" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="77"/>
-      <c r="B29" s="78"/>
-      <c r="C29" s="78"/>
-      <c r="D29" s="78"/>
-      <c r="E29" s="78"/>
-      <c r="F29" s="78"/>
-      <c r="G29" s="79"/>
+      <c r="A29" s="62"/>
+      <c r="B29" s="63"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="63"/>
+      <c r="G29" s="64"/>
       <c r="N29" s="6"/>
     </row>
     <row r="30" spans="1:14" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="77"/>
-      <c r="B30" s="78"/>
-      <c r="C30" s="78"/>
-      <c r="D30" s="78"/>
-      <c r="E30" s="78"/>
-      <c r="F30" s="78"/>
-      <c r="G30" s="79"/>
+      <c r="A30" s="62"/>
+      <c r="B30" s="63"/>
+      <c r="C30" s="63"/>
+      <c r="D30" s="63"/>
+      <c r="E30" s="63"/>
+      <c r="F30" s="63"/>
+      <c r="G30" s="64"/>
       <c r="N30" s="6"/>
     </row>
     <row r="31" spans="1:14" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="83"/>
-      <c r="B31" s="84"/>
-      <c r="C31" s="84"/>
-      <c r="D31" s="84"/>
-      <c r="E31" s="84"/>
-      <c r="F31" s="84"/>
-      <c r="G31" s="85"/>
+      <c r="A31" s="68"/>
+      <c r="B31" s="69"/>
+      <c r="C31" s="69"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="69"/>
+      <c r="G31" s="70"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
@@ -1884,6 +1867,12 @@
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="F15:G15"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="A16:B16"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="B3:D3"/>
@@ -1898,12 +1887,6 @@
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="A27:G27"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="A16:B16"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{7CAA0989-4F43-4FD8-B312-70CA488ABB3B}">

</xml_diff>

<commit_message>
excel source file layout changed
</commit_message>
<xml_diff>
--- a/public/6 R Daily Report.xlsx
+++ b/public/6 R Daily Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyunmyung.kim\workspace\React\exbon-daily-report\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20155C8-04A3-4398-BC5F-B7EEEB58E8C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11EC3C02-C3D1-4679-B42E-170BDF35C2A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,6 +574,48 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
@@ -627,48 +669,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1179,24 +1179,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="29.42578125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="7" style="4" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="27.140625" style="4" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" style="4" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
       <c r="F1" s="28"/>
       <c r="G1" s="2"/>
     </row>
@@ -1204,11 +1204,11 @@
       <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="56"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="38"/>
       <c r="E2" s="19" t="s">
         <v>3</v>
       </c>
@@ -1220,11 +1220,11 @@
       <c r="A3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="56"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="38"/>
       <c r="E3" s="20" t="s">
         <v>6</v>
       </c>
@@ -1236,11 +1236,11 @@
       <c r="A4" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="65"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="47"/>
       <c r="E4" s="20" t="s">
         <v>20</v>
       </c>
@@ -1250,43 +1250,43 @@
       <c r="A5" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="54"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="56"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="38"/>
       <c r="E5" s="20" t="s">
         <v>21</v>
       </c>
       <c r="F5" s="32"/>
     </row>
     <row r="6" spans="1:15" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="61" t="s">
+      <c r="C6" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="62"/>
-      <c r="E6" s="43" t="s">
+      <c r="D6" s="44"/>
+      <c r="E6" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="59" t="s">
+      <c r="F6" s="41" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:15" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="58"/>
-      <c r="B7" s="60"/>
+      <c r="A7" s="40"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="21" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="44"/>
-      <c r="F7" s="60"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="42"/>
     </row>
     <row r="8" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="26"/>
@@ -1354,155 +1354,155 @@
       <c r="F15" s="25"/>
     </row>
     <row r="16" spans="1:15" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="50" t="s">
+      <c r="A16" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="51"/>
+      <c r="B16" s="65"/>
       <c r="C16" s="14">
         <f>SUM(C8:C15)</f>
         <v>0</v>
       </c>
       <c r="D16" s="18"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="46"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="60"/>
       <c r="M16" s="15"/>
       <c r="N16" s="16"/>
       <c r="O16" s="16"/>
     </row>
     <row r="17" spans="1:13" s="5" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="47" t="s">
+      <c r="A17" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="48"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="49"/>
+      <c r="B17" s="62"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="63"/>
       <c r="M17" s="6"/>
     </row>
     <row r="18" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="34"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="36"/>
+      <c r="A18" s="48"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="50"/>
       <c r="M18" s="6"/>
     </row>
     <row r="19" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="37"/>
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="39"/>
+      <c r="A19" s="51"/>
+      <c r="B19" s="52"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="53"/>
       <c r="M19" s="6"/>
     </row>
     <row r="20" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="37"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="39"/>
+      <c r="A20" s="51"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="53"/>
     </row>
     <row r="21" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="40"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="42"/>
+      <c r="A21" s="54"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="56"/>
     </row>
     <row r="22" spans="1:13" s="5" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="47" t="s">
+      <c r="A22" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="48"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="48"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="49"/>
+      <c r="B22" s="62"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="63"/>
       <c r="M22" s="6"/>
     </row>
     <row r="23" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="34"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="36"/>
+      <c r="A23" s="48"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="50"/>
       <c r="M23" s="6"/>
     </row>
     <row r="24" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="37"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="39"/>
+      <c r="A24" s="51"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="53"/>
     </row>
     <row r="25" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="37"/>
-      <c r="B25" s="38"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="39"/>
+      <c r="A25" s="51"/>
+      <c r="B25" s="52"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="53"/>
     </row>
     <row r="26" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="40"/>
-      <c r="B26" s="41"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="42"/>
+      <c r="A26" s="54"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="56"/>
     </row>
     <row r="27" spans="1:13" s="5" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="47" t="s">
+      <c r="A27" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="48"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="49"/>
+      <c r="B27" s="62"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="62"/>
+      <c r="E27" s="62"/>
+      <c r="F27" s="63"/>
       <c r="M27" s="6"/>
     </row>
     <row r="28" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="34"/>
-      <c r="B28" s="35"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="36"/>
+      <c r="A28" s="48"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="50"/>
       <c r="M28" s="6"/>
     </row>
     <row r="29" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="37"/>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="39"/>
+      <c r="A29" s="51"/>
+      <c r="B29" s="52"/>
+      <c r="C29" s="52"/>
+      <c r="D29" s="52"/>
+      <c r="E29" s="52"/>
+      <c r="F29" s="53"/>
       <c r="M29" s="6"/>
     </row>
     <row r="30" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="37"/>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="39"/>
+      <c r="A30" s="51"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="53"/>
       <c r="M30" s="6"/>
     </row>
     <row r="31" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="40"/>
-      <c r="B31" s="41"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="42"/>
+      <c r="A31" s="54"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="56"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
@@ -1560,14 +1560,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B5:D5"/>
     <mergeCell ref="A18:F21"/>
     <mergeCell ref="A23:F26"/>
     <mergeCell ref="A28:F31"/>
@@ -1578,6 +1570,14 @@
     <mergeCell ref="A27:F27"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="F6:F7"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B5:D5"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{7CAA0989-4F43-4FD8-B312-70CA488ABB3B}">
@@ -1585,7 +1585,7 @@
     </dataValidation>
   </dataValidations>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
form layout changed again
</commit_message>
<xml_diff>
--- a/public/6 R Daily Report.xlsx
+++ b/public/6 R Daily Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyunmyung.kim\workspace\React\exbon-daily-report\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11EC3C02-C3D1-4679-B42E-170BDF35C2A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB9F4F3-F8FE-4294-B377-97384B93E7E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,6 +574,66 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -595,12 +655,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -615,60 +669,6 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -802,9 +802,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
+      <xdr:colOff>95250</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1476375" cy="428625"/>
     <xdr:pic>
@@ -837,7 +837,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4924425" y="114300"/>
+          <a:off x="4095750" y="123825"/>
           <a:ext cx="1476375" cy="428625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1174,29 +1174,29 @@
   <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="7" style="4" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="27.140625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="6" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" style="4" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" style="4" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
       <c r="F1" s="28"/>
       <c r="G1" s="2"/>
     </row>
@@ -1204,11 +1204,11 @@
       <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="38"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="58"/>
       <c r="E2" s="19" t="s">
         <v>3</v>
       </c>
@@ -1220,11 +1220,11 @@
       <c r="A3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="38"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="58"/>
       <c r="E3" s="20" t="s">
         <v>6</v>
       </c>
@@ -1236,11 +1236,11 @@
       <c r="A4" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="46"/>
-      <c r="D4" s="47"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="65"/>
       <c r="E4" s="20" t="s">
         <v>20</v>
       </c>
@@ -1250,43 +1250,43 @@
       <c r="A5" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="38"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="58"/>
       <c r="E5" s="20" t="s">
         <v>21</v>
       </c>
       <c r="F5" s="32"/>
     </row>
     <row r="6" spans="1:15" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="44"/>
-      <c r="E6" s="57" t="s">
+      <c r="D6" s="62"/>
+      <c r="E6" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="41" t="s">
+      <c r="F6" s="52" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:15" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="40"/>
-      <c r="B7" s="42"/>
+      <c r="A7" s="60"/>
+      <c r="B7" s="53"/>
       <c r="C7" s="21" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="58"/>
-      <c r="F7" s="42"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="53"/>
     </row>
     <row r="8" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="26"/>
@@ -1354,155 +1354,155 @@
       <c r="F15" s="25"/>
     </row>
     <row r="16" spans="1:15" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="64" t="s">
+      <c r="A16" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="65"/>
+      <c r="B16" s="51"/>
       <c r="C16" s="14">
         <f>SUM(C8:C15)</f>
         <v>0</v>
       </c>
       <c r="D16" s="18"/>
-      <c r="E16" s="59"/>
-      <c r="F16" s="60"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="46"/>
       <c r="M16" s="15"/>
       <c r="N16" s="16"/>
       <c r="O16" s="16"/>
     </row>
     <row r="17" spans="1:13" s="5" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="61" t="s">
+      <c r="A17" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="62"/>
-      <c r="C17" s="62"/>
-      <c r="D17" s="62"/>
-      <c r="E17" s="62"/>
-      <c r="F17" s="63"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="49"/>
       <c r="M17" s="6"/>
     </row>
     <row r="18" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="48"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="50"/>
+      <c r="A18" s="34"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="36"/>
       <c r="M18" s="6"/>
     </row>
     <row r="19" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="51"/>
-      <c r="B19" s="52"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="53"/>
+      <c r="A19" s="37"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="39"/>
       <c r="M19" s="6"/>
     </row>
     <row r="20" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="51"/>
-      <c r="B20" s="52"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="53"/>
+      <c r="A20" s="37"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="39"/>
     </row>
     <row r="21" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="54"/>
-      <c r="B21" s="55"/>
-      <c r="C21" s="55"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="56"/>
+      <c r="A21" s="40"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="42"/>
     </row>
     <row r="22" spans="1:13" s="5" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="61" t="s">
+      <c r="A22" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="62"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="63"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="49"/>
       <c r="M22" s="6"/>
     </row>
     <row r="23" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="48"/>
-      <c r="B23" s="49"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="50"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="36"/>
       <c r="M23" s="6"/>
     </row>
     <row r="24" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="51"/>
-      <c r="B24" s="52"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="53"/>
+      <c r="A24" s="37"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="39"/>
     </row>
     <row r="25" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="51"/>
-      <c r="B25" s="52"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="52"/>
-      <c r="F25" s="53"/>
+      <c r="A25" s="37"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="39"/>
     </row>
     <row r="26" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="54"/>
-      <c r="B26" s="55"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="56"/>
+      <c r="A26" s="40"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="42"/>
     </row>
     <row r="27" spans="1:13" s="5" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="61" t="s">
+      <c r="A27" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="62"/>
-      <c r="C27" s="62"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="62"/>
-      <c r="F27" s="63"/>
+      <c r="B27" s="48"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="49"/>
       <c r="M27" s="6"/>
     </row>
     <row r="28" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="48"/>
-      <c r="B28" s="49"/>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="50"/>
+      <c r="A28" s="34"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="36"/>
       <c r="M28" s="6"/>
     </row>
     <row r="29" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="51"/>
-      <c r="B29" s="52"/>
-      <c r="C29" s="52"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="52"/>
-      <c r="F29" s="53"/>
+      <c r="A29" s="37"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="39"/>
       <c r="M29" s="6"/>
     </row>
     <row r="30" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="51"/>
-      <c r="B30" s="52"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="53"/>
+      <c r="A30" s="37"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="39"/>
       <c r="M30" s="6"/>
     </row>
     <row r="31" spans="1:13" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="54"/>
-      <c r="B31" s="55"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="55"/>
-      <c r="E31" s="55"/>
-      <c r="F31" s="56"/>
+      <c r="A31" s="40"/>
+      <c r="B31" s="41"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="42"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
@@ -1560,6 +1560,14 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B5:D5"/>
     <mergeCell ref="A18:F21"/>
     <mergeCell ref="A23:F26"/>
     <mergeCell ref="A28:F31"/>
@@ -1570,14 +1578,6 @@
     <mergeCell ref="A27:F27"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="F6:F7"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B5:D5"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{7CAA0989-4F43-4FD8-B312-70CA488ABB3B}">

</xml_diff>

<commit_message>
test success form fixed
</commit_message>
<xml_diff>
--- a/public/6 R Daily Report.xlsx
+++ b/public/6 R Daily Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyunmyung.kim\workspace\React\exbon-daily-report\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3BE762B-D53B-4509-8E0E-C519E331FEF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A71CEC-55AD-45A0-96B3-78307CA90AEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -144,7 +144,7 @@
     </font>
     <font>
       <b/>
-      <sz val="20"/>
+      <sz val="14"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -562,16 +562,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -797,6 +797,54 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>533401</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1213908" cy="352425"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{371CE15E-ACBC-4819-82D6-7E5E416202DB}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{0D9A761D-5D17-4A17-A5D6-0D1475E85A58}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3228976" y="142875"/>
+          <a:ext cx="1213908" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
@@ -1131,12 +1179,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="6" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" style="4" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" style="4" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
@@ -1164,7 +1212,7 @@
       <c r="E2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="32" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1180,7 +1228,7 @@
       <c r="E3" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="32" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1196,10 +1244,10 @@
       <c r="E4" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="32"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="5" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="30" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="56"/>
@@ -1208,7 +1256,7 @@
       <c r="E5" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5" s="33"/>
     </row>
     <row r="6" spans="1:15" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="59" t="s">
@@ -1228,7 +1276,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" s="3" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="60"/>
       <c r="B7" s="53"/>
       <c r="C7" s="21" t="s">
@@ -1537,7 +1585,7 @@
     </dataValidation>
   </dataValidations>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId2"/>

</xml_diff>